<commit_message>
[Draw schematic for the display unit #8]
committing pin assignment for N5150M8CD
</commit_message>
<xml_diff>
--- a/Eagles/EPaperDisplayUnit/pin_assignment.xlsx
+++ b/Eagles/EPaperDisplayUnit/pin_assignment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Pin Name</t>
   </si>
@@ -98,6 +98,33 @@
   </si>
   <si>
     <t>Alternative</t>
+  </si>
+  <si>
+    <t>N5150M8CD</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>F5</t>
   </si>
 </sst>
 </file>
@@ -439,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F14"/>
+  <dimension ref="B4:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,9 +478,10 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -469,8 +497,11 @@
       <c r="F4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -486,8 +517,11 @@
       <c r="F5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -503,8 +537,11 @@
       <c r="F6">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -520,8 +557,11 @@
       <c r="F7">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -537,8 +577,11 @@
       <c r="F8">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -554,8 +597,11 @@
       <c r="F9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -571,8 +617,11 @@
       <c r="F10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -588,8 +637,11 @@
       <c r="F11">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -605,8 +657,11 @@
       <c r="F12">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -617,7 +672,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>17</v>
       </c>

</xml_diff>